<commit_message>
Update from recent findings
</commit_message>
<xml_diff>
--- a/out/money_per_project.xlsx
+++ b/out/money_per_project.xlsx
@@ -14106,10 +14106,10 @@
         <v>0</v>
       </c>
       <c r="I89" t="n">
-        <v>2600000</v>
+        <v>100000</v>
       </c>
       <c r="J89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K89" t="n">
         <v>1000000</v>
@@ -30584,10 +30584,10 @@
         <v>0</v>
       </c>
       <c r="I196" t="n">
-        <v>12000000</v>
+        <v>0</v>
       </c>
       <c r="J196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K196" t="n">
         <v>250000</v>

</xml_diff>